<commit_message>
Update 18.03.25 - Adding files for setup.py
</commit_message>
<xml_diff>
--- a/res/efficiency_cal/230724_Eff_Cal_EastHPGe_Lab35.xlsx
+++ b/res/efficiency_cal/230724_Eff_Cal_EastHPGe_Lab35.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\_Staff folders\RE22\1_Projects\6_Gamma spectrometry\Efficiency function\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renald_e\Documents\monitor-xs-ip2\res\efficiency_cal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E52039-D8B9-4D35-840A-48E1821899E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6F061E-B16A-476A-9F87-F6C03BC294A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MeasureData" sheetId="3" r:id="rId1"/>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D3463F-72DF-4D03-8C09-AD3118C4BF8A}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:AB1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>